<commit_message>
Completion of Vector Diagram
This commit has the completion of the vector diagram, as well as the addition of the Data Dictionary Spread Sheet. This spread sheet will have definitions for each table in the tab.
</commit_message>
<xml_diff>
--- a/Copy of Description of the Log Files.xlsx
+++ b/Copy of Description of the Log Files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd2a091fe8f62e20/ARA/2019S1/DBM/Assignment1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd2a091fe8f62e20/ARA/2019S1/DBM/Assignment1/DBAssignment2019-S1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{C78B9CD7-4686-47D1-ACBA-191AD168683E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{547FDF02-4DC8-4981-A429-A133EB5CB0E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_8BBB71BDE09D5BFA1468A4841D1072D1C5A995FD" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34755" yWindow="315" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,8 +495,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +522,17 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -525,15 +543,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -946,19 +968,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="71" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.265625" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -972,7 +994,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -989,7 +1011,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1006,7 +1028,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1023,7 +1045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1040,7 +1062,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1057,284 +1079,284 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="4">
         <v>6</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="4">
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="4">
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="4">
         <v>-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="4">
         <v>0</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="4">
         <v>-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="4">
         <v>-5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="4">
         <v>0</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="4">
         <v>-6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>0</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="4">
         <v>-7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>0</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="4">
         <v>46.066666666666698</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1345,7 +1367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1356,7 +1378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1367,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1389,7 +1411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1400,62 +1422,62 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="33" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="34" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    <row r="36" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+    <row r="37" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -1466,7 +1488,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -1477,7 +1499,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -1488,7 +1510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1499,7 +1521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1510,62 +1532,62 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
@@ -1576,7 +1598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -1587,7 +1609,7 @@
         <v>152.97191476123101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -1598,7 +1620,7 @@
         <v>-27.0792295037818</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
@@ -1609,7 +1631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>64</v>
       </c>
@@ -1620,7 +1642,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1631,7 +1653,7 @@
         <v>8.93144040002811E+19</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -1642,7 +1664,7 @@
         <v>8.9610180002248999E+19</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -1653,7 +1675,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>70</v>
       </c>
@@ -1664,7 +1686,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>72</v>
       </c>
@@ -1675,7 +1697,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>74</v>
       </c>
@@ -1686,7 +1708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>76</v>
       </c>
@@ -1697,7 +1719,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>77</v>
       </c>
@@ -1708,58 +1730,58 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    <row r="61" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+    <row r="62" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+    <row r="63" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
+    <row r="64" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    <row r="65" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="3" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completion of ERD and Table Creation Script
</commit_message>
<xml_diff>
--- a/Copy of Description of the Log Files.xlsx
+++ b/Copy of Description of the Log Files.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="11_8BBB71BDE09D5BFA1468A4841D1072D1C5A995FD" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34755" yWindow="315" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="15389" windowHeight="9532" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -968,19 +968,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.1328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -994,7 +994,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>21</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
         <v>22</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
         <v>23</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>24</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>46.066666666666698</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>29</v>
       </c>
@@ -1345,7 +1345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>30</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1367,7 +1367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="4" t="s">
         <v>37</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="4" t="s">
         <v>39</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="4" t="s">
         <v>41</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A37" s="4" t="s">
         <v>43</v>
       </c>
@@ -1477,7 +1477,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A38" s="2" t="s">
         <v>44</v>
       </c>
@@ -1488,7 +1488,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A39" s="2" t="s">
         <v>46</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="2" t="s">
         <v>49</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="2" t="s">
         <v>50</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A43" s="2" t="s">
         <v>51</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="2" t="s">
         <v>53</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="2" t="s">
         <v>54</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>56</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="2" t="s">
         <v>57</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A49" s="2" t="s">
         <v>60</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>152.97191476123101</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>-27.0792295037818</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A51" s="2" t="s">
         <v>62</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A52" s="2" t="s">
         <v>64</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>8.93144040002811E+19</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>67</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>8.9610180002248999E+19</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>68</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A56" s="2" t="s">
         <v>70</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A57" s="2" t="s">
         <v>72</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A58" s="2" t="s">
         <v>74</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A59" s="2" t="s">
         <v>76</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A60" s="2" t="s">
         <v>77</v>
       </c>
@@ -1730,7 +1730,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A61" s="3" t="s">
         <v>79</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A62" s="3" t="s">
         <v>81</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A63" s="3" t="s">
         <v>82</v>
       </c>
@@ -1763,7 +1763,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A64" s="3" t="s">
         <v>84</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A65" s="3" t="s">
         <v>85</v>
       </c>

</xml_diff>